<commit_message>
updated the README to be more descriptive
</commit_message>
<xml_diff>
--- a/Tools/ChecklistComparisons/TERM_TBC_MIATE_Comparison_040622.xlsx
+++ b/Tools/ChecklistComparisons/TERM_TBC_MIATE_Comparison_040622.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/MIATE/Tools/ChecklistComparisons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="8_{EACA5486-EEE5-4AF2-8C89-D6DBD37B18BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47BC8CC6-CBDC-43DC-B42A-AAC8EA0CB116}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="8_{EACA5486-EEE5-4AF2-8C89-D6DBD37B18BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3B74CB4-5F7B-4D7B-9C50-04D3AF132C53}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5CA93EF9-461D-42A8-9208-D042D8A1AB7B}"/>
+    <workbookView minimized="1" xWindow="2955" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5CA93EF9-461D-42A8-9208-D042D8A1AB7B}"/>
   </bookViews>
   <sheets>
     <sheet name="GlobalComparison" sheetId="1" r:id="rId1"/>
@@ -7971,10 +7971,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447A0621-05D8-46CB-A783-63232CE3D10C}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O139" sqref="O139"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8068,7 +8069,7 @@
       </c>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="98" t="s">
         <v>15</v>
       </c>
@@ -8115,7 +8116,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="99" t="s">
         <v>17</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="99" t="s">
         <v>19</v>
       </c>
@@ -8209,7 +8210,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="99" t="s">
         <v>22</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="99" t="s">
         <v>29</v>
       </c>
@@ -8299,7 +8300,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="99" t="s">
         <v>31</v>
       </c>
@@ -8344,7 +8345,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="99" t="s">
         <v>32</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="10" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99" t="s">
         <v>34</v>
       </c>
@@ -8435,7 +8436,7 @@
       </c>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="99" t="s">
         <v>35</v>
       </c>
@@ -8478,7 +8479,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="99" t="s">
         <v>36</v>
       </c>
@@ -8521,7 +8522,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="99" t="s">
         <v>38</v>
       </c>
@@ -8564,7 +8565,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="99" t="s">
         <v>39</v>
       </c>
@@ -8607,7 +8608,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="99" t="s">
         <v>40</v>
       </c>
@@ -8650,7 +8651,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="99" t="s">
         <v>41</v>
       </c>
@@ -8693,7 +8694,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="99" t="s">
         <v>42</v>
       </c>
@@ -8736,7 +8737,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="99" t="s">
         <v>43</v>
       </c>
@@ -8779,7 +8780,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="99" t="s">
         <v>44</v>
       </c>
@@ -8822,7 +8823,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="99" t="s">
         <v>45</v>
       </c>
@@ -8865,7 +8866,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="99" t="s">
         <v>46</v>
       </c>
@@ -8908,7 +8909,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="99" t="s">
         <v>47</v>
       </c>
@@ -8951,7 +8952,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="99" t="s">
         <v>48</v>
       </c>
@@ -8994,7 +8995,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="99" t="s">
         <v>51</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="99" t="s">
         <v>53</v>
       </c>
@@ -9080,7 +9081,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="99" t="s">
         <v>54</v>
       </c>
@@ -9123,7 +9124,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>55</v>
       </c>
@@ -9166,7 +9167,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="99" t="s">
         <v>56</v>
       </c>
@@ -9209,7 +9210,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="99" t="s">
         <v>58</v>
       </c>
@@ -9254,7 +9255,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="99" t="s">
         <v>59</v>
       </c>
@@ -9299,7 +9300,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="99" t="s">
         <v>60</v>
       </c>
@@ -9342,7 +9343,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="99" t="s">
         <v>61</v>
       </c>
@@ -9387,7 +9388,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="99" t="s">
         <v>62</v>
       </c>
@@ -9430,7 +9431,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="99" t="s">
         <v>63</v>
       </c>
@@ -9473,7 +9474,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="99" t="s">
         <v>64</v>
       </c>
@@ -9516,7 +9517,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="99" t="s">
         <v>66</v>
       </c>
@@ -9563,7 +9564,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="99" t="s">
         <v>67</v>
       </c>
@@ -9610,7 +9611,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="99" t="s">
         <v>68</v>
       </c>
@@ -9702,7 +9703,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="29.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="99" t="s">
         <v>72</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="99" t="s">
         <v>73</v>
       </c>
@@ -9796,7 +9797,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="99" t="s">
         <v>74</v>
       </c>
@@ -9843,7 +9844,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="99" t="s">
         <v>75</v>
       </c>
@@ -9890,7 +9891,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="99" t="s">
         <v>76</v>
       </c>
@@ -9933,7 +9934,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="99" t="s">
         <v>78</v>
       </c>
@@ -9980,7 +9981,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="99" t="s">
         <v>79</v>
       </c>
@@ -10023,7 +10024,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="99" t="s">
         <v>80</v>
       </c>
@@ -10066,7 +10067,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="99" t="s">
         <v>81</v>
       </c>
@@ -10109,7 +10110,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="99" t="s">
         <v>82</v>
       </c>
@@ -10152,7 +10153,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="99" t="s">
         <v>78</v>
       </c>
@@ -10199,7 +10200,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="99"/>
       <c r="B51" s="95"/>
       <c r="C51" s="96" t="s">
@@ -10242,7 +10243,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="99"/>
       <c r="B52" s="95"/>
       <c r="C52" s="96" t="s">
@@ -10285,7 +10286,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="99"/>
       <c r="B53" s="95"/>
       <c r="C53" s="96" t="s">
@@ -10328,7 +10329,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="99"/>
       <c r="B54" s="95"/>
       <c r="C54" s="96"/>
@@ -10371,7 +10372,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="99"/>
       <c r="B55" s="95"/>
       <c r="C55" s="96"/>
@@ -10414,7 +10415,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="99" t="s">
         <v>96</v>
       </c>
@@ -10457,7 +10458,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="99" t="s">
         <v>97</v>
       </c>
@@ -10502,7 +10503,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="99" t="s">
         <v>98</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="99" t="s">
         <v>99</v>
       </c>
@@ -10592,7 +10593,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="99" t="s">
         <v>101</v>
       </c>
@@ -10635,7 +10636,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="99" t="s">
         <v>102</v>
       </c>
@@ -10680,7 +10681,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="99" t="s">
         <v>103</v>
       </c>
@@ -10725,7 +10726,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="99" t="s">
         <v>105</v>
       </c>
@@ -10772,7 +10773,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="99" t="s">
         <v>106</v>
       </c>
@@ -10819,7 +10820,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="99" t="s">
         <v>107</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="99"/>
       <c r="B66" s="95"/>
       <c r="C66" s="96"/>
@@ -10905,7 +10906,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="99"/>
       <c r="B67" s="95"/>
       <c r="C67" s="96"/>
@@ -10948,7 +10949,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="99"/>
       <c r="B68" s="95"/>
       <c r="C68" s="96"/>
@@ -10991,7 +10992,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="99"/>
       <c r="B69" s="95"/>
       <c r="C69" s="96"/>
@@ -11034,7 +11035,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="99" t="s">
         <v>134</v>
       </c>
@@ -11081,7 +11082,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="99" t="s">
         <v>136</v>
       </c>
@@ -11128,7 +11129,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="99"/>
       <c r="B72" s="95"/>
       <c r="C72" s="96"/>
@@ -11171,7 +11172,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="99" t="s">
         <v>145</v>
       </c>
@@ -11214,7 +11215,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="100" t="s">
         <v>147</v>
       </c>
@@ -11257,7 +11258,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="100" t="s">
         <v>149</v>
       </c>
@@ -11302,7 +11303,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="100" t="s">
         <v>151</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="100" t="s">
         <v>154</v>
       </c>
@@ -11388,7 +11389,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="101" t="s">
         <v>155</v>
       </c>
@@ -11431,7 +11432,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="99" t="s">
         <v>157</v>
       </c>
@@ -11474,7 +11475,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="99" t="s">
         <v>159</v>
       </c>
@@ -11517,7 +11518,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="99" t="s">
         <v>161</v>
       </c>
@@ -11560,7 +11561,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="99" t="s">
         <v>173</v>
       </c>
@@ -11603,7 +11604,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="99" t="s">
         <v>174</v>
       </c>
@@ -11646,7 +11647,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="99" t="s">
         <v>175</v>
       </c>
@@ -11689,7 +11690,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="101" t="s">
         <v>178</v>
       </c>
@@ -11736,7 +11737,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="101" t="s">
         <v>182</v>
       </c>
@@ -11779,7 +11780,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="99" t="s">
         <v>187</v>
       </c>
@@ -11822,7 +11823,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="99" t="s">
         <v>188</v>
       </c>
@@ -11865,7 +11866,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="99" t="s">
         <v>189</v>
       </c>
@@ -11908,7 +11909,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="99" t="s">
         <v>190</v>
       </c>
@@ -11951,7 +11952,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="99" t="s">
         <v>191</v>
       </c>
@@ -11994,7 +11995,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="99" t="s">
         <v>192</v>
       </c>
@@ -12037,7 +12038,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="99" t="s">
         <v>193</v>
       </c>
@@ -12080,7 +12081,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="99" t="s">
         <v>194</v>
       </c>
@@ -12123,7 +12124,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="99" t="s">
         <v>195</v>
       </c>
@@ -12166,7 +12167,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="99" t="s">
         <v>196</v>
       </c>
@@ -12209,7 +12210,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="99" t="s">
         <v>198</v>
       </c>
@@ -12252,7 +12253,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="99" t="s">
         <v>199</v>
       </c>
@@ -12295,7 +12296,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="99" t="s">
         <v>200</v>
       </c>
@@ -12338,7 +12339,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="99" t="s">
         <v>201</v>
       </c>
@@ -12381,7 +12382,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="99" t="s">
         <v>203</v>
       </c>
@@ -12424,7 +12425,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="99" t="s">
         <v>205</v>
       </c>
@@ -12467,7 +12468,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="16.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="16.7" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="99" t="s">
         <v>206</v>
       </c>
@@ -12510,7 +12511,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="104" spans="1:17" s="19" customFormat="1" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" s="19" customFormat="1" ht="29.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="99" t="s">
         <v>207</v>
       </c>
@@ -12554,7 +12555,7 @@
       </c>
       <c r="Q104" s="1"/>
     </row>
-    <row r="105" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="99" t="s">
         <v>209</v>
       </c>
@@ -12601,7 +12602,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="99" t="s">
         <v>210</v>
       </c>
@@ -12644,7 +12645,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="99" t="s">
         <v>211</v>
       </c>
@@ -12687,7 +12688,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="99" t="s">
         <v>212</v>
       </c>
@@ -12730,7 +12731,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="99" t="s">
         <v>214</v>
       </c>
@@ -12773,7 +12774,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="99" t="s">
         <v>215</v>
       </c>
@@ -12820,7 +12821,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="99" t="s">
         <v>216</v>
       </c>
@@ -12863,7 +12864,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="102" t="s">
         <v>219</v>
       </c>
@@ -12908,7 +12909,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="102" t="s">
         <v>220</v>
       </c>
@@ -12953,7 +12954,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="102" t="s">
         <v>229</v>
       </c>
@@ -12998,7 +12999,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="102" t="s">
         <v>231</v>
       </c>
@@ -13041,7 +13042,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="102" t="s">
         <v>233</v>
       </c>
@@ -13088,7 +13089,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="102"/>
       <c r="B117" s="95"/>
       <c r="C117" s="96" t="s">
@@ -13412,6 +13413,13 @@
       <c r="M144" s="107"/>
     </row>
   </sheetData>
+  <autoFilter ref="G2:M118" xr:uid="{447A0621-05D8-46CB-A783-63232CE3D10C}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="O50">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>

</xml_diff>